<commit_message>
essai d'ajout d'un filedialog
</commit_message>
<xml_diff>
--- a/src/listedepoints.xlsx
+++ b/src/listedepoints.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npelleschi\Documents\DOSSIER\7-Code\SYSCOPACK\DEFPTS\src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Liste" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Libellé</t>
   </si>
@@ -36,50 +31,14 @@
     <t>Télé-Commande</t>
   </si>
   <si>
-    <t xml:space="preserve">Chaudière 1 Défaut pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 1 Commande pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 1 Fin de course V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 1 Commande V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 2 Défaut pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 2 Commande pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 2 Fin de course V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 2 Commande V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 3 Défaut pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 3 Commande pompe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 3 Fin de course V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaudière 3 Commande V2V </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TOTAUX (12 points)</t>
+    <t xml:space="preserve"> TOTAUX (0 points)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,15 +54,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,12 +65,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,29 +81,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -199,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,10 +168,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,7 +202,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,20 +377,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
     <col min="2" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,225 +405,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="E2" s="1">
         <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction problème select file box
</commit_message>
<xml_diff>
--- a/src/listedepoints.xlsx
+++ b/src/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Libellé</t>
   </si>
@@ -31,14 +31,38 @@
     <t>Télé-Commande</t>
   </si>
   <si>
-    <t xml:space="preserve"> TOTAUX (0 points)</t>
+    <t xml:space="preserve">Chaudière 1 Défaut pompe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 1 Commande pompe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 1 Fin de course V2V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 1 Commande V2V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 2 Défaut pompe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 2 Commande pompe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 2 Fin de course V2V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaudière 2 Commande V2V </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TOTAUX (8 points)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +78,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -65,6 +96,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -81,9 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,20 +444,156 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>